<commit_message>
Rerun TODE grade norms with correct minRaw
</commit_message>
<xml_diff>
--- a/OUTPUT-FILES/NORMS/TODE_8.27.21_fornorms/lswe_sum-raw-ss-lookup-tabbed-grade.xlsx
+++ b/OUTPUT-FILES/NORMS/TODE_8.27.21_fornorms/lswe_sum-raw-ss-lookup-tabbed-grade.xlsx
@@ -356,7 +356,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B60"/>
+  <dimension ref="A1:B40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -376,473 +376,313 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>-20</v>
+        <v>0</v>
       </c>
       <c r="B2">
-        <v>40</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3">
       <c r="A3">
-        <v>-19</v>
+        <v>1</v>
       </c>
       <c r="B3">
-        <v>40</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4">
       <c r="A4">
-        <v>-18</v>
+        <v>2</v>
       </c>
       <c r="B4">
-        <v>40</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5">
       <c r="A5">
-        <v>-17</v>
+        <v>3</v>
       </c>
       <c r="B5">
-        <v>40</v>
+        <v>73</v>
       </c>
     </row>
     <row r="6">
       <c r="A6">
-        <v>-16</v>
+        <v>4</v>
       </c>
       <c r="B6">
-        <v>40</v>
+        <v>75</v>
       </c>
     </row>
     <row r="7">
       <c r="A7">
-        <v>-15</v>
+        <v>5</v>
       </c>
       <c r="B7">
-        <v>40</v>
+        <v>78</v>
       </c>
     </row>
     <row r="8">
       <c r="A8">
-        <v>-14</v>
+        <v>6</v>
       </c>
       <c r="B8">
-        <v>40</v>
+        <v>80</v>
       </c>
     </row>
     <row r="9">
       <c r="A9">
-        <v>-13</v>
+        <v>7</v>
       </c>
       <c r="B9">
-        <v>40</v>
+        <v>82</v>
       </c>
     </row>
     <row r="10">
       <c r="A10">
-        <v>-12</v>
+        <v>8</v>
       </c>
       <c r="B10">
-        <v>40</v>
+        <v>85</v>
       </c>
     </row>
     <row r="11">
       <c r="A11">
-        <v>-11</v>
+        <v>9</v>
       </c>
       <c r="B11">
-        <v>40</v>
+        <v>87</v>
       </c>
     </row>
     <row r="12">
       <c r="A12">
-        <v>-10</v>
+        <v>10</v>
       </c>
       <c r="B12">
-        <v>42</v>
+        <v>90</v>
       </c>
     </row>
     <row r="13">
       <c r="A13">
-        <v>-9</v>
+        <v>11</v>
       </c>
       <c r="B13">
-        <v>44</v>
+        <v>92</v>
       </c>
     </row>
     <row r="14">
       <c r="A14">
-        <v>-8</v>
+        <v>12</v>
       </c>
       <c r="B14">
-        <v>46</v>
+        <v>94</v>
       </c>
     </row>
     <row r="15">
       <c r="A15">
-        <v>-7</v>
+        <v>13</v>
       </c>
       <c r="B15">
-        <v>49</v>
+        <v>97</v>
       </c>
     </row>
     <row r="16">
       <c r="A16">
-        <v>-6</v>
+        <v>14</v>
       </c>
       <c r="B16">
-        <v>51</v>
+        <v>99</v>
       </c>
     </row>
     <row r="17">
       <c r="A17">
-        <v>-5</v>
+        <v>15</v>
       </c>
       <c r="B17">
-        <v>54</v>
+        <v>102</v>
       </c>
     </row>
     <row r="18">
       <c r="A18">
-        <v>-4</v>
+        <v>16</v>
       </c>
       <c r="B18">
-        <v>56</v>
+        <v>104</v>
       </c>
     </row>
     <row r="19">
       <c r="A19">
-        <v>-3</v>
+        <v>17</v>
       </c>
       <c r="B19">
-        <v>58</v>
+        <v>106</v>
       </c>
     </row>
     <row r="20">
       <c r="A20">
-        <v>-2</v>
+        <v>18</v>
       </c>
       <c r="B20">
-        <v>61</v>
+        <v>109</v>
       </c>
     </row>
     <row r="21">
       <c r="A21">
-        <v>-1</v>
+        <v>19</v>
       </c>
       <c r="B21">
-        <v>63</v>
+        <v>111</v>
       </c>
     </row>
     <row r="22">
       <c r="A22">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="B22">
-        <v>66</v>
+        <v>114</v>
       </c>
     </row>
     <row r="23">
       <c r="A23">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="B23">
-        <v>68</v>
+        <v>116</v>
       </c>
     </row>
     <row r="24">
       <c r="A24">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="B24">
-        <v>70</v>
+        <v>118</v>
       </c>
     </row>
     <row r="25">
       <c r="A25">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="B25">
-        <v>73</v>
+        <v>121</v>
       </c>
     </row>
     <row r="26">
       <c r="A26">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="B26">
-        <v>75</v>
+        <v>123</v>
       </c>
     </row>
     <row r="27">
       <c r="A27">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="B27">
-        <v>78</v>
+        <v>126</v>
       </c>
     </row>
     <row r="28">
       <c r="A28">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="B28">
-        <v>80</v>
+        <v>128</v>
       </c>
     </row>
     <row r="29">
       <c r="A29">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="B29">
-        <v>82</v>
+        <v>130</v>
       </c>
     </row>
     <row r="30">
       <c r="A30">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="B30">
-        <v>85</v>
+        <v>130</v>
       </c>
     </row>
     <row r="31">
       <c r="A31">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="B31">
-        <v>87</v>
+        <v>130</v>
       </c>
     </row>
     <row r="32">
       <c r="A32">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="B32">
-        <v>90</v>
+        <v>130</v>
       </c>
     </row>
     <row r="33">
       <c r="A33">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="B33">
-        <v>92</v>
+        <v>130</v>
       </c>
     </row>
     <row r="34">
       <c r="A34">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="B34">
-        <v>94</v>
+        <v>130</v>
       </c>
     </row>
     <row r="35">
       <c r="A35">
-        <v>13</v>
+        <v>33</v>
       </c>
       <c r="B35">
-        <v>97</v>
+        <v>130</v>
       </c>
     </row>
     <row r="36">
       <c r="A36">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="B36">
-        <v>99</v>
+        <v>130</v>
       </c>
     </row>
     <row r="37">
       <c r="A37">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="B37">
-        <v>102</v>
+        <v>130</v>
       </c>
     </row>
     <row r="38">
       <c r="A38">
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="B38">
-        <v>104</v>
+        <v>130</v>
       </c>
     </row>
     <row r="39">
       <c r="A39">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="B39">
-        <v>106</v>
+        <v>130</v>
       </c>
     </row>
     <row r="40">
       <c r="A40">
-        <v>18</v>
+        <v>38</v>
       </c>
       <c r="B40">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41">
-        <v>19</v>
-      </c>
-      <c r="B41">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42">
-        <v>20</v>
-      </c>
-      <c r="B42">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43">
-        <v>21</v>
-      </c>
-      <c r="B43">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44">
-        <v>22</v>
-      </c>
-      <c r="B44">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45">
-        <v>23</v>
-      </c>
-      <c r="B45">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46">
-        <v>24</v>
-      </c>
-      <c r="B46">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47">
-        <v>25</v>
-      </c>
-      <c r="B47">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48">
-        <v>26</v>
-      </c>
-      <c r="B48">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49">
-        <v>27</v>
-      </c>
-      <c r="B49">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50">
-        <v>28</v>
-      </c>
-      <c r="B50">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51">
-        <v>29</v>
-      </c>
-      <c r="B51">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52">
-        <v>30</v>
-      </c>
-      <c r="B52">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53">
-        <v>31</v>
-      </c>
-      <c r="B53">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54">
-        <v>32</v>
-      </c>
-      <c r="B54">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55">
-        <v>33</v>
-      </c>
-      <c r="B55">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56">
-        <v>34</v>
-      </c>
-      <c r="B56">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57">
-        <v>35</v>
-      </c>
-      <c r="B57">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58">
-        <v>36</v>
-      </c>
-      <c r="B58">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59">
-        <v>37</v>
-      </c>
-      <c r="B59">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60">
-        <v>38</v>
-      </c>
-      <c r="B60">
         <v>130</v>
       </c>
     </row>
@@ -853,7 +693,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B60"/>
+  <dimension ref="A1:B40"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -873,473 +713,313 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>-20</v>
+        <v>0</v>
       </c>
       <c r="B2">
-        <v>40</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3">
       <c r="A3">
-        <v>-19</v>
+        <v>1</v>
       </c>
       <c r="B3">
-        <v>40</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4">
       <c r="A4">
-        <v>-18</v>
+        <v>2</v>
       </c>
       <c r="B4">
-        <v>40</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5">
       <c r="A5">
-        <v>-17</v>
+        <v>3</v>
       </c>
       <c r="B5">
-        <v>40</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6">
       <c r="A6">
-        <v>-16</v>
+        <v>4</v>
       </c>
       <c r="B6">
-        <v>40</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7">
       <c r="A7">
-        <v>-15</v>
+        <v>5</v>
       </c>
       <c r="B7">
-        <v>40</v>
+        <v>67</v>
       </c>
     </row>
     <row r="8">
       <c r="A8">
-        <v>-14</v>
+        <v>6</v>
       </c>
       <c r="B8">
-        <v>40</v>
+        <v>70</v>
       </c>
     </row>
     <row r="9">
       <c r="A9">
-        <v>-13</v>
+        <v>7</v>
       </c>
       <c r="B9">
-        <v>40</v>
+        <v>72</v>
       </c>
     </row>
     <row r="10">
       <c r="A10">
-        <v>-12</v>
+        <v>8</v>
       </c>
       <c r="B10">
-        <v>40</v>
+        <v>74</v>
       </c>
     </row>
     <row r="11">
       <c r="A11">
-        <v>-11</v>
+        <v>9</v>
       </c>
       <c r="B11">
-        <v>40</v>
+        <v>77</v>
       </c>
     </row>
     <row r="12">
       <c r="A12">
-        <v>-10</v>
+        <v>10</v>
       </c>
       <c r="B12">
-        <v>40</v>
+        <v>79</v>
       </c>
     </row>
     <row r="13">
       <c r="A13">
-        <v>-9</v>
+        <v>11</v>
       </c>
       <c r="B13">
-        <v>40</v>
+        <v>82</v>
       </c>
     </row>
     <row r="14">
       <c r="A14">
-        <v>-8</v>
+        <v>12</v>
       </c>
       <c r="B14">
-        <v>40</v>
+        <v>84</v>
       </c>
     </row>
     <row r="15">
       <c r="A15">
-        <v>-7</v>
+        <v>13</v>
       </c>
       <c r="B15">
-        <v>40</v>
+        <v>86</v>
       </c>
     </row>
     <row r="16">
       <c r="A16">
-        <v>-6</v>
+        <v>14</v>
       </c>
       <c r="B16">
-        <v>41</v>
+        <v>89</v>
       </c>
     </row>
     <row r="17">
       <c r="A17">
-        <v>-5</v>
+        <v>15</v>
       </c>
       <c r="B17">
-        <v>43</v>
+        <v>91</v>
       </c>
     </row>
     <row r="18">
       <c r="A18">
-        <v>-4</v>
+        <v>16</v>
       </c>
       <c r="B18">
-        <v>45</v>
+        <v>94</v>
       </c>
     </row>
     <row r="19">
       <c r="A19">
-        <v>-3</v>
+        <v>17</v>
       </c>
       <c r="B19">
-        <v>48</v>
+        <v>96</v>
       </c>
     </row>
     <row r="20">
       <c r="A20">
-        <v>-2</v>
+        <v>18</v>
       </c>
       <c r="B20">
-        <v>50</v>
+        <v>98</v>
       </c>
     </row>
     <row r="21">
       <c r="A21">
-        <v>-1</v>
+        <v>19</v>
       </c>
       <c r="B21">
-        <v>53</v>
+        <v>101</v>
       </c>
     </row>
     <row r="22">
       <c r="A22">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="B22">
-        <v>55</v>
+        <v>103</v>
       </c>
     </row>
     <row r="23">
       <c r="A23">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="B23">
-        <v>57</v>
+        <v>106</v>
       </c>
     </row>
     <row r="24">
       <c r="A24">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="B24">
-        <v>60</v>
+        <v>108</v>
       </c>
     </row>
     <row r="25">
       <c r="A25">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="B25">
-        <v>62</v>
+        <v>110</v>
       </c>
     </row>
     <row r="26">
       <c r="A26">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="B26">
-        <v>65</v>
+        <v>113</v>
       </c>
     </row>
     <row r="27">
       <c r="A27">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="B27">
-        <v>67</v>
+        <v>115</v>
       </c>
     </row>
     <row r="28">
       <c r="A28">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="B28">
-        <v>70</v>
+        <v>118</v>
       </c>
     </row>
     <row r="29">
       <c r="A29">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="B29">
-        <v>72</v>
+        <v>120</v>
       </c>
     </row>
     <row r="30">
       <c r="A30">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="B30">
-        <v>74</v>
+        <v>122</v>
       </c>
     </row>
     <row r="31">
       <c r="A31">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="B31">
-        <v>77</v>
+        <v>125</v>
       </c>
     </row>
     <row r="32">
       <c r="A32">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="B32">
-        <v>79</v>
+        <v>127</v>
       </c>
     </row>
     <row r="33">
       <c r="A33">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="B33">
-        <v>82</v>
+        <v>130</v>
       </c>
     </row>
     <row r="34">
       <c r="A34">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="B34">
-        <v>84</v>
+        <v>130</v>
       </c>
     </row>
     <row r="35">
       <c r="A35">
-        <v>13</v>
+        <v>33</v>
       </c>
       <c r="B35">
-        <v>86</v>
+        <v>130</v>
       </c>
     </row>
     <row r="36">
       <c r="A36">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="B36">
-        <v>89</v>
+        <v>130</v>
       </c>
     </row>
     <row r="37">
       <c r="A37">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="B37">
-        <v>91</v>
+        <v>130</v>
       </c>
     </row>
     <row r="38">
       <c r="A38">
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="B38">
-        <v>94</v>
+        <v>130</v>
       </c>
     </row>
     <row r="39">
       <c r="A39">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="B39">
-        <v>96</v>
+        <v>130</v>
       </c>
     </row>
     <row r="40">
       <c r="A40">
-        <v>18</v>
+        <v>38</v>
       </c>
       <c r="B40">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41">
-        <v>19</v>
-      </c>
-      <c r="B41">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42">
-        <v>20</v>
-      </c>
-      <c r="B42">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43">
-        <v>21</v>
-      </c>
-      <c r="B43">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44">
-        <v>22</v>
-      </c>
-      <c r="B44">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45">
-        <v>23</v>
-      </c>
-      <c r="B45">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46">
-        <v>24</v>
-      </c>
-      <c r="B46">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47">
-        <v>25</v>
-      </c>
-      <c r="B47">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48">
-        <v>26</v>
-      </c>
-      <c r="B48">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49">
-        <v>27</v>
-      </c>
-      <c r="B49">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50">
-        <v>28</v>
-      </c>
-      <c r="B50">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51">
-        <v>29</v>
-      </c>
-      <c r="B51">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52">
-        <v>30</v>
-      </c>
-      <c r="B52">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53">
-        <v>31</v>
-      </c>
-      <c r="B53">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54">
-        <v>32</v>
-      </c>
-      <c r="B54">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55">
-        <v>33</v>
-      </c>
-      <c r="B55">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56">
-        <v>34</v>
-      </c>
-      <c r="B56">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57">
-        <v>35</v>
-      </c>
-      <c r="B57">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58">
-        <v>36</v>
-      </c>
-      <c r="B58">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59">
-        <v>37</v>
-      </c>
-      <c r="B59">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60">
-        <v>38</v>
-      </c>
-      <c r="B60">
         <v>130</v>
       </c>
     </row>
@@ -1350,7 +1030,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B60"/>
+  <dimension ref="A1:B40"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1370,473 +1050,313 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>-20</v>
+        <v>0</v>
       </c>
       <c r="B2">
-        <v>40</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3">
       <c r="A3">
-        <v>-19</v>
+        <v>1</v>
       </c>
       <c r="B3">
-        <v>40</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4">
       <c r="A4">
-        <v>-18</v>
+        <v>2</v>
       </c>
       <c r="B4">
-        <v>40</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5">
       <c r="A5">
-        <v>-17</v>
+        <v>3</v>
       </c>
       <c r="B5">
-        <v>40</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6">
       <c r="A6">
-        <v>-16</v>
+        <v>4</v>
       </c>
       <c r="B6">
-        <v>40</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7">
       <c r="A7">
-        <v>-15</v>
+        <v>5</v>
       </c>
       <c r="B7">
-        <v>40</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8">
       <c r="A8">
-        <v>-14</v>
+        <v>6</v>
       </c>
       <c r="B8">
-        <v>40</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9">
       <c r="A9">
-        <v>-13</v>
+        <v>7</v>
       </c>
       <c r="B9">
-        <v>40</v>
+        <v>61</v>
       </c>
     </row>
     <row r="10">
       <c r="A10">
-        <v>-12</v>
+        <v>8</v>
       </c>
       <c r="B10">
-        <v>40</v>
+        <v>64</v>
       </c>
     </row>
     <row r="11">
       <c r="A11">
-        <v>-11</v>
+        <v>9</v>
       </c>
       <c r="B11">
-        <v>40</v>
+        <v>66</v>
       </c>
     </row>
     <row r="12">
       <c r="A12">
-        <v>-10</v>
+        <v>10</v>
       </c>
       <c r="B12">
-        <v>40</v>
+        <v>69</v>
       </c>
     </row>
     <row r="13">
       <c r="A13">
-        <v>-9</v>
+        <v>11</v>
       </c>
       <c r="B13">
-        <v>40</v>
+        <v>71</v>
       </c>
     </row>
     <row r="14">
       <c r="A14">
-        <v>-8</v>
+        <v>12</v>
       </c>
       <c r="B14">
-        <v>40</v>
+        <v>73</v>
       </c>
     </row>
     <row r="15">
       <c r="A15">
-        <v>-7</v>
+        <v>13</v>
       </c>
       <c r="B15">
-        <v>40</v>
+        <v>76</v>
       </c>
     </row>
     <row r="16">
       <c r="A16">
-        <v>-6</v>
+        <v>14</v>
       </c>
       <c r="B16">
-        <v>40</v>
+        <v>78</v>
       </c>
     </row>
     <row r="17">
       <c r="A17">
-        <v>-5</v>
+        <v>15</v>
       </c>
       <c r="B17">
-        <v>40</v>
+        <v>81</v>
       </c>
     </row>
     <row r="18">
       <c r="A18">
-        <v>-4</v>
+        <v>16</v>
       </c>
       <c r="B18">
-        <v>40</v>
+        <v>83</v>
       </c>
     </row>
     <row r="19">
       <c r="A19">
-        <v>-3</v>
+        <v>17</v>
       </c>
       <c r="B19">
-        <v>40</v>
+        <v>85</v>
       </c>
     </row>
     <row r="20">
       <c r="A20">
-        <v>-2</v>
+        <v>18</v>
       </c>
       <c r="B20">
-        <v>40</v>
+        <v>88</v>
       </c>
     </row>
     <row r="21">
       <c r="A21">
-        <v>-1</v>
+        <v>19</v>
       </c>
       <c r="B21">
-        <v>42</v>
+        <v>90</v>
       </c>
     </row>
     <row r="22">
       <c r="A22">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="B22">
-        <v>45</v>
+        <v>93</v>
       </c>
     </row>
     <row r="23">
       <c r="A23">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="B23">
-        <v>47</v>
+        <v>95</v>
       </c>
     </row>
     <row r="24">
       <c r="A24">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="B24">
-        <v>49</v>
+        <v>97</v>
       </c>
     </row>
     <row r="25">
       <c r="A25">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="B25">
-        <v>52</v>
+        <v>100</v>
       </c>
     </row>
     <row r="26">
       <c r="A26">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="B26">
-        <v>54</v>
+        <v>102</v>
       </c>
     </row>
     <row r="27">
       <c r="A27">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="B27">
-        <v>57</v>
+        <v>105</v>
       </c>
     </row>
     <row r="28">
       <c r="A28">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="B28">
-        <v>59</v>
+        <v>107</v>
       </c>
     </row>
     <row r="29">
       <c r="A29">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="B29">
-        <v>61</v>
+        <v>110</v>
       </c>
     </row>
     <row r="30">
       <c r="A30">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="B30">
-        <v>64</v>
+        <v>112</v>
       </c>
     </row>
     <row r="31">
       <c r="A31">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="B31">
-        <v>66</v>
+        <v>114</v>
       </c>
     </row>
     <row r="32">
       <c r="A32">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="B32">
-        <v>69</v>
+        <v>117</v>
       </c>
     </row>
     <row r="33">
       <c r="A33">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="B33">
-        <v>71</v>
+        <v>119</v>
       </c>
     </row>
     <row r="34">
       <c r="A34">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="B34">
-        <v>73</v>
+        <v>122</v>
       </c>
     </row>
     <row r="35">
       <c r="A35">
-        <v>13</v>
+        <v>33</v>
       </c>
       <c r="B35">
-        <v>76</v>
+        <v>124</v>
       </c>
     </row>
     <row r="36">
       <c r="A36">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="B36">
-        <v>78</v>
+        <v>126</v>
       </c>
     </row>
     <row r="37">
       <c r="A37">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="B37">
-        <v>81</v>
+        <v>129</v>
       </c>
     </row>
     <row r="38">
       <c r="A38">
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="B38">
-        <v>83</v>
+        <v>130</v>
       </c>
     </row>
     <row r="39">
       <c r="A39">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="B39">
-        <v>85</v>
+        <v>130</v>
       </c>
     </row>
     <row r="40">
       <c r="A40">
-        <v>18</v>
+        <v>38</v>
       </c>
       <c r="B40">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41">
-        <v>19</v>
-      </c>
-      <c r="B41">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42">
-        <v>20</v>
-      </c>
-      <c r="B42">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43">
-        <v>21</v>
-      </c>
-      <c r="B43">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44">
-        <v>22</v>
-      </c>
-      <c r="B44">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45">
-        <v>23</v>
-      </c>
-      <c r="B45">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46">
-        <v>24</v>
-      </c>
-      <c r="B46">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47">
-        <v>25</v>
-      </c>
-      <c r="B47">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48">
-        <v>26</v>
-      </c>
-      <c r="B48">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49">
-        <v>27</v>
-      </c>
-      <c r="B49">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50">
-        <v>28</v>
-      </c>
-      <c r="B50">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51">
-        <v>29</v>
-      </c>
-      <c r="B51">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52">
-        <v>30</v>
-      </c>
-      <c r="B52">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53">
-        <v>31</v>
-      </c>
-      <c r="B53">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54">
-        <v>32</v>
-      </c>
-      <c r="B54">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55">
-        <v>33</v>
-      </c>
-      <c r="B55">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56">
-        <v>34</v>
-      </c>
-      <c r="B56">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57">
-        <v>35</v>
-      </c>
-      <c r="B57">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58">
-        <v>36</v>
-      </c>
-      <c r="B58">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59">
-        <v>37</v>
-      </c>
-      <c r="B59">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60">
-        <v>38</v>
-      </c>
-      <c r="B60">
         <v>130</v>
       </c>
     </row>
@@ -1847,7 +1367,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B60"/>
+  <dimension ref="A1:B40"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1867,473 +1387,313 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>-20</v>
+        <v>0</v>
       </c>
       <c r="B2">
-        <v>40</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3">
       <c r="A3">
-        <v>-19</v>
+        <v>1</v>
       </c>
       <c r="B3">
-        <v>40</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4">
       <c r="A4">
-        <v>-18</v>
+        <v>2</v>
       </c>
       <c r="B4">
-        <v>40</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5">
       <c r="A5">
-        <v>-17</v>
+        <v>3</v>
       </c>
       <c r="B5">
-        <v>40</v>
+        <v>73</v>
       </c>
     </row>
     <row r="6">
       <c r="A6">
-        <v>-16</v>
+        <v>4</v>
       </c>
       <c r="B6">
-        <v>40</v>
+        <v>75</v>
       </c>
     </row>
     <row r="7">
       <c r="A7">
-        <v>-15</v>
+        <v>5</v>
       </c>
       <c r="B7">
-        <v>40</v>
+        <v>78</v>
       </c>
     </row>
     <row r="8">
       <c r="A8">
-        <v>-14</v>
+        <v>6</v>
       </c>
       <c r="B8">
-        <v>40</v>
+        <v>80</v>
       </c>
     </row>
     <row r="9">
       <c r="A9">
-        <v>-13</v>
+        <v>7</v>
       </c>
       <c r="B9">
-        <v>40</v>
+        <v>82</v>
       </c>
     </row>
     <row r="10">
       <c r="A10">
-        <v>-12</v>
+        <v>8</v>
       </c>
       <c r="B10">
-        <v>40</v>
+        <v>85</v>
       </c>
     </row>
     <row r="11">
       <c r="A11">
-        <v>-11</v>
+        <v>9</v>
       </c>
       <c r="B11">
-        <v>40</v>
+        <v>87</v>
       </c>
     </row>
     <row r="12">
       <c r="A12">
-        <v>-10</v>
+        <v>10</v>
       </c>
       <c r="B12">
-        <v>42</v>
+        <v>90</v>
       </c>
     </row>
     <row r="13">
       <c r="A13">
-        <v>-9</v>
+        <v>11</v>
       </c>
       <c r="B13">
-        <v>44</v>
+        <v>92</v>
       </c>
     </row>
     <row r="14">
       <c r="A14">
-        <v>-8</v>
+        <v>12</v>
       </c>
       <c r="B14">
-        <v>46</v>
+        <v>94</v>
       </c>
     </row>
     <row r="15">
       <c r="A15">
-        <v>-7</v>
+        <v>13</v>
       </c>
       <c r="B15">
-        <v>49</v>
+        <v>97</v>
       </c>
     </row>
     <row r="16">
       <c r="A16">
-        <v>-6</v>
+        <v>14</v>
       </c>
       <c r="B16">
-        <v>51</v>
+        <v>99</v>
       </c>
     </row>
     <row r="17">
       <c r="A17">
-        <v>-5</v>
+        <v>15</v>
       </c>
       <c r="B17">
-        <v>54</v>
+        <v>102</v>
       </c>
     </row>
     <row r="18">
       <c r="A18">
-        <v>-4</v>
+        <v>16</v>
       </c>
       <c r="B18">
-        <v>56</v>
+        <v>104</v>
       </c>
     </row>
     <row r="19">
       <c r="A19">
-        <v>-3</v>
+        <v>17</v>
       </c>
       <c r="B19">
-        <v>58</v>
+        <v>106</v>
       </c>
     </row>
     <row r="20">
       <c r="A20">
-        <v>-2</v>
+        <v>18</v>
       </c>
       <c r="B20">
-        <v>61</v>
+        <v>109</v>
       </c>
     </row>
     <row r="21">
       <c r="A21">
-        <v>-1</v>
+        <v>19</v>
       </c>
       <c r="B21">
-        <v>63</v>
+        <v>111</v>
       </c>
     </row>
     <row r="22">
       <c r="A22">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="B22">
-        <v>66</v>
+        <v>114</v>
       </c>
     </row>
     <row r="23">
       <c r="A23">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="B23">
-        <v>68</v>
+        <v>116</v>
       </c>
     </row>
     <row r="24">
       <c r="A24">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="B24">
-        <v>70</v>
+        <v>118</v>
       </c>
     </row>
     <row r="25">
       <c r="A25">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="B25">
-        <v>73</v>
+        <v>121</v>
       </c>
     </row>
     <row r="26">
       <c r="A26">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="B26">
-        <v>75</v>
+        <v>123</v>
       </c>
     </row>
     <row r="27">
       <c r="A27">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="B27">
-        <v>78</v>
+        <v>126</v>
       </c>
     </row>
     <row r="28">
       <c r="A28">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="B28">
-        <v>80</v>
+        <v>128</v>
       </c>
     </row>
     <row r="29">
       <c r="A29">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="B29">
-        <v>82</v>
+        <v>130</v>
       </c>
     </row>
     <row r="30">
       <c r="A30">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="B30">
-        <v>85</v>
+        <v>130</v>
       </c>
     </row>
     <row r="31">
       <c r="A31">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="B31">
-        <v>87</v>
+        <v>130</v>
       </c>
     </row>
     <row r="32">
       <c r="A32">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="B32">
-        <v>90</v>
+        <v>130</v>
       </c>
     </row>
     <row r="33">
       <c r="A33">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="B33">
-        <v>92</v>
+        <v>130</v>
       </c>
     </row>
     <row r="34">
       <c r="A34">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="B34">
-        <v>94</v>
+        <v>130</v>
       </c>
     </row>
     <row r="35">
       <c r="A35">
-        <v>13</v>
+        <v>33</v>
       </c>
       <c r="B35">
-        <v>97</v>
+        <v>130</v>
       </c>
     </row>
     <row r="36">
       <c r="A36">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="B36">
-        <v>99</v>
+        <v>130</v>
       </c>
     </row>
     <row r="37">
       <c r="A37">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="B37">
-        <v>102</v>
+        <v>130</v>
       </c>
     </row>
     <row r="38">
       <c r="A38">
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="B38">
-        <v>104</v>
+        <v>130</v>
       </c>
     </row>
     <row r="39">
       <c r="A39">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="B39">
-        <v>106</v>
+        <v>130</v>
       </c>
     </row>
     <row r="40">
       <c r="A40">
-        <v>18</v>
+        <v>38</v>
       </c>
       <c r="B40">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41">
-        <v>19</v>
-      </c>
-      <c r="B41">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42">
-        <v>20</v>
-      </c>
-      <c r="B42">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43">
-        <v>21</v>
-      </c>
-      <c r="B43">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44">
-        <v>22</v>
-      </c>
-      <c r="B44">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45">
-        <v>23</v>
-      </c>
-      <c r="B45">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46">
-        <v>24</v>
-      </c>
-      <c r="B46">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47">
-        <v>25</v>
-      </c>
-      <c r="B47">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48">
-        <v>26</v>
-      </c>
-      <c r="B48">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49">
-        <v>27</v>
-      </c>
-      <c r="B49">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50">
-        <v>28</v>
-      </c>
-      <c r="B50">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51">
-        <v>29</v>
-      </c>
-      <c r="B51">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52">
-        <v>30</v>
-      </c>
-      <c r="B52">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53">
-        <v>31</v>
-      </c>
-      <c r="B53">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54">
-        <v>32</v>
-      </c>
-      <c r="B54">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55">
-        <v>33</v>
-      </c>
-      <c r="B55">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56">
-        <v>34</v>
-      </c>
-      <c r="B56">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57">
-        <v>35</v>
-      </c>
-      <c r="B57">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58">
-        <v>36</v>
-      </c>
-      <c r="B58">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59">
-        <v>37</v>
-      </c>
-      <c r="B59">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60">
-        <v>38</v>
-      </c>
-      <c r="B60">
         <v>130</v>
       </c>
     </row>
@@ -2344,7 +1704,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B60"/>
+  <dimension ref="A1:B40"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2364,7 +1724,7 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>-20</v>
+        <v>0</v>
       </c>
       <c r="B2">
         <v>40</v>
@@ -2372,7 +1732,7 @@
     </row>
     <row r="3">
       <c r="A3">
-        <v>-19</v>
+        <v>1</v>
       </c>
       <c r="B3">
         <v>40</v>
@@ -2380,7 +1740,7 @@
     </row>
     <row r="4">
       <c r="A4">
-        <v>-18</v>
+        <v>2</v>
       </c>
       <c r="B4">
         <v>40</v>
@@ -2388,7 +1748,7 @@
     </row>
     <row r="5">
       <c r="A5">
-        <v>-17</v>
+        <v>3</v>
       </c>
       <c r="B5">
         <v>40</v>
@@ -2396,7 +1756,7 @@
     </row>
     <row r="6">
       <c r="A6">
-        <v>-16</v>
+        <v>4</v>
       </c>
       <c r="B6">
         <v>40</v>
@@ -2404,7 +1764,7 @@
     </row>
     <row r="7">
       <c r="A7">
-        <v>-15</v>
+        <v>5</v>
       </c>
       <c r="B7">
         <v>40</v>
@@ -2412,7 +1772,7 @@
     </row>
     <row r="8">
       <c r="A8">
-        <v>-14</v>
+        <v>6</v>
       </c>
       <c r="B8">
         <v>40</v>
@@ -2420,7 +1780,7 @@
     </row>
     <row r="9">
       <c r="A9">
-        <v>-13</v>
+        <v>7</v>
       </c>
       <c r="B9">
         <v>40</v>
@@ -2428,409 +1788,249 @@
     </row>
     <row r="10">
       <c r="A10">
-        <v>-12</v>
+        <v>8</v>
       </c>
       <c r="B10">
-        <v>40</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11">
       <c r="A11">
-        <v>-11</v>
+        <v>9</v>
       </c>
       <c r="B11">
-        <v>40</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12">
       <c r="A12">
-        <v>-10</v>
+        <v>10</v>
       </c>
       <c r="B12">
-        <v>40</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13">
       <c r="A13">
-        <v>-9</v>
+        <v>11</v>
       </c>
       <c r="B13">
-        <v>40</v>
+        <v>50</v>
       </c>
     </row>
     <row r="14">
       <c r="A14">
-        <v>-8</v>
+        <v>12</v>
       </c>
       <c r="B14">
-        <v>40</v>
+        <v>52</v>
       </c>
     </row>
     <row r="15">
       <c r="A15">
-        <v>-7</v>
+        <v>13</v>
       </c>
       <c r="B15">
-        <v>40</v>
+        <v>55</v>
       </c>
     </row>
     <row r="16">
       <c r="A16">
-        <v>-6</v>
+        <v>14</v>
       </c>
       <c r="B16">
-        <v>40</v>
+        <v>57</v>
       </c>
     </row>
     <row r="17">
       <c r="A17">
-        <v>-5</v>
+        <v>15</v>
       </c>
       <c r="B17">
-        <v>40</v>
+        <v>60</v>
       </c>
     </row>
     <row r="18">
       <c r="A18">
-        <v>-4</v>
+        <v>16</v>
       </c>
       <c r="B18">
-        <v>40</v>
+        <v>62</v>
       </c>
     </row>
     <row r="19">
       <c r="A19">
-        <v>-3</v>
+        <v>17</v>
       </c>
       <c r="B19">
-        <v>40</v>
+        <v>65</v>
       </c>
     </row>
     <row r="20">
       <c r="A20">
-        <v>-2</v>
+        <v>18</v>
       </c>
       <c r="B20">
-        <v>40</v>
+        <v>67</v>
       </c>
     </row>
     <row r="21">
       <c r="A21">
-        <v>-1</v>
+        <v>19</v>
       </c>
       <c r="B21">
-        <v>40</v>
+        <v>69</v>
       </c>
     </row>
     <row r="22">
       <c r="A22">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="B22">
-        <v>40</v>
+        <v>72</v>
       </c>
     </row>
     <row r="23">
       <c r="A23">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="B23">
-        <v>40</v>
+        <v>74</v>
       </c>
     </row>
     <row r="24">
       <c r="A24">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="B24">
-        <v>40</v>
+        <v>77</v>
       </c>
     </row>
     <row r="25">
       <c r="A25">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="B25">
-        <v>40</v>
+        <v>79</v>
       </c>
     </row>
     <row r="26">
       <c r="A26">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="B26">
-        <v>40</v>
+        <v>81</v>
       </c>
     </row>
     <row r="27">
       <c r="A27">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="B27">
-        <v>40</v>
+        <v>84</v>
       </c>
     </row>
     <row r="28">
       <c r="A28">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="B28">
-        <v>40</v>
+        <v>86</v>
       </c>
     </row>
     <row r="29">
       <c r="A29">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="B29">
-        <v>40</v>
+        <v>89</v>
       </c>
     </row>
     <row r="30">
       <c r="A30">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="B30">
-        <v>43</v>
+        <v>91</v>
       </c>
     </row>
     <row r="31">
       <c r="A31">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="B31">
-        <v>45</v>
+        <v>93</v>
       </c>
     </row>
     <row r="32">
       <c r="A32">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="B32">
-        <v>48</v>
+        <v>96</v>
       </c>
     </row>
     <row r="33">
       <c r="A33">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="B33">
-        <v>50</v>
+        <v>98</v>
       </c>
     </row>
     <row r="34">
       <c r="A34">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="B34">
-        <v>52</v>
+        <v>101</v>
       </c>
     </row>
     <row r="35">
       <c r="A35">
-        <v>13</v>
+        <v>33</v>
       </c>
       <c r="B35">
-        <v>55</v>
+        <v>103</v>
       </c>
     </row>
     <row r="36">
       <c r="A36">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="B36">
-        <v>57</v>
+        <v>105</v>
       </c>
     </row>
     <row r="37">
       <c r="A37">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="B37">
-        <v>60</v>
+        <v>108</v>
       </c>
     </row>
     <row r="38">
       <c r="A38">
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="B38">
-        <v>62</v>
+        <v>110</v>
       </c>
     </row>
     <row r="39">
       <c r="A39">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="B39">
-        <v>65</v>
+        <v>113</v>
       </c>
     </row>
     <row r="40">
       <c r="A40">
-        <v>18</v>
+        <v>38</v>
       </c>
       <c r="B40">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41">
-        <v>19</v>
-      </c>
-      <c r="B41">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42">
-        <v>20</v>
-      </c>
-      <c r="B42">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43">
-        <v>21</v>
-      </c>
-      <c r="B43">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44">
-        <v>22</v>
-      </c>
-      <c r="B44">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45">
-        <v>23</v>
-      </c>
-      <c r="B45">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46">
-        <v>24</v>
-      </c>
-      <c r="B46">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47">
-        <v>25</v>
-      </c>
-      <c r="B47">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48">
-        <v>26</v>
-      </c>
-      <c r="B48">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49">
-        <v>27</v>
-      </c>
-      <c r="B49">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50">
-        <v>28</v>
-      </c>
-      <c r="B50">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51">
-        <v>29</v>
-      </c>
-      <c r="B51">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52">
-        <v>30</v>
-      </c>
-      <c r="B52">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53">
-        <v>31</v>
-      </c>
-      <c r="B53">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54">
-        <v>32</v>
-      </c>
-      <c r="B54">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55">
-        <v>33</v>
-      </c>
-      <c r="B55">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56">
-        <v>34</v>
-      </c>
-      <c r="B56">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57">
-        <v>35</v>
-      </c>
-      <c r="B57">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58">
-        <v>36</v>
-      </c>
-      <c r="B58">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59">
-        <v>37</v>
-      </c>
-      <c r="B59">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60">
-        <v>38</v>
-      </c>
-      <c r="B60">
         <v>115</v>
       </c>
     </row>
@@ -2841,7 +2041,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B60"/>
+  <dimension ref="A1:B40"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2861,7 +2061,7 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>-20</v>
+        <v>0</v>
       </c>
       <c r="B2">
         <v>40</v>
@@ -2869,7 +2069,7 @@
     </row>
     <row r="3">
       <c r="A3">
-        <v>-19</v>
+        <v>1</v>
       </c>
       <c r="B3">
         <v>40</v>
@@ -2877,7 +2077,7 @@
     </row>
     <row r="4">
       <c r="A4">
-        <v>-18</v>
+        <v>2</v>
       </c>
       <c r="B4">
         <v>40</v>
@@ -2885,7 +2085,7 @@
     </row>
     <row r="5">
       <c r="A5">
-        <v>-17</v>
+        <v>3</v>
       </c>
       <c r="B5">
         <v>40</v>
@@ -2893,7 +2093,7 @@
     </row>
     <row r="6">
       <c r="A6">
-        <v>-16</v>
+        <v>4</v>
       </c>
       <c r="B6">
         <v>40</v>
@@ -2901,7 +2101,7 @@
     </row>
     <row r="7">
       <c r="A7">
-        <v>-15</v>
+        <v>5</v>
       </c>
       <c r="B7">
         <v>40</v>
@@ -2909,7 +2109,7 @@
     </row>
     <row r="8">
       <c r="A8">
-        <v>-14</v>
+        <v>6</v>
       </c>
       <c r="B8">
         <v>40</v>
@@ -2917,7 +2117,7 @@
     </row>
     <row r="9">
       <c r="A9">
-        <v>-13</v>
+        <v>7</v>
       </c>
       <c r="B9">
         <v>40</v>
@@ -2925,7 +2125,7 @@
     </row>
     <row r="10">
       <c r="A10">
-        <v>-12</v>
+        <v>8</v>
       </c>
       <c r="B10">
         <v>40</v>
@@ -2933,7 +2133,7 @@
     </row>
     <row r="11">
       <c r="A11">
-        <v>-11</v>
+        <v>9</v>
       </c>
       <c r="B11">
         <v>40</v>
@@ -2941,7 +2141,7 @@
     </row>
     <row r="12">
       <c r="A12">
-        <v>-10</v>
+        <v>10</v>
       </c>
       <c r="B12">
         <v>40</v>
@@ -2949,7 +2149,7 @@
     </row>
     <row r="13">
       <c r="A13">
-        <v>-9</v>
+        <v>11</v>
       </c>
       <c r="B13">
         <v>40</v>
@@ -2957,377 +2157,217 @@
     </row>
     <row r="14">
       <c r="A14">
-        <v>-8</v>
+        <v>12</v>
       </c>
       <c r="B14">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="15">
       <c r="A15">
-        <v>-7</v>
+        <v>13</v>
       </c>
       <c r="B15">
-        <v>40</v>
+        <v>44</v>
       </c>
     </row>
     <row r="16">
       <c r="A16">
-        <v>-6</v>
+        <v>14</v>
       </c>
       <c r="B16">
-        <v>40</v>
+        <v>47</v>
       </c>
     </row>
     <row r="17">
       <c r="A17">
-        <v>-5</v>
+        <v>15</v>
       </c>
       <c r="B17">
-        <v>40</v>
+        <v>49</v>
       </c>
     </row>
     <row r="18">
       <c r="A18">
-        <v>-4</v>
+        <v>16</v>
       </c>
       <c r="B18">
-        <v>40</v>
+        <v>52</v>
       </c>
     </row>
     <row r="19">
       <c r="A19">
-        <v>-3</v>
+        <v>17</v>
       </c>
       <c r="B19">
-        <v>40</v>
+        <v>54</v>
       </c>
     </row>
     <row r="20">
       <c r="A20">
-        <v>-2</v>
+        <v>18</v>
       </c>
       <c r="B20">
-        <v>40</v>
+        <v>56</v>
       </c>
     </row>
     <row r="21">
       <c r="A21">
-        <v>-1</v>
+        <v>19</v>
       </c>
       <c r="B21">
-        <v>40</v>
+        <v>59</v>
       </c>
     </row>
     <row r="22">
       <c r="A22">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="B22">
-        <v>40</v>
+        <v>61</v>
       </c>
     </row>
     <row r="23">
       <c r="A23">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="B23">
-        <v>40</v>
+        <v>64</v>
       </c>
     </row>
     <row r="24">
       <c r="A24">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="B24">
-        <v>40</v>
+        <v>66</v>
       </c>
     </row>
     <row r="25">
       <c r="A25">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="B25">
-        <v>40</v>
+        <v>68</v>
       </c>
     </row>
     <row r="26">
       <c r="A26">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="B26">
-        <v>40</v>
+        <v>71</v>
       </c>
     </row>
     <row r="27">
       <c r="A27">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="B27">
-        <v>40</v>
+        <v>73</v>
       </c>
     </row>
     <row r="28">
       <c r="A28">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="B28">
-        <v>40</v>
+        <v>76</v>
       </c>
     </row>
     <row r="29">
       <c r="A29">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="B29">
-        <v>40</v>
+        <v>78</v>
       </c>
     </row>
     <row r="30">
       <c r="A30">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="B30">
-        <v>40</v>
+        <v>80</v>
       </c>
     </row>
     <row r="31">
       <c r="A31">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="B31">
-        <v>40</v>
+        <v>83</v>
       </c>
     </row>
     <row r="32">
       <c r="A32">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="B32">
-        <v>40</v>
+        <v>85</v>
       </c>
     </row>
     <row r="33">
       <c r="A33">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="B33">
-        <v>40</v>
+        <v>88</v>
       </c>
     </row>
     <row r="34">
       <c r="A34">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="B34">
-        <v>42</v>
+        <v>90</v>
       </c>
     </row>
     <row r="35">
       <c r="A35">
-        <v>13</v>
+        <v>33</v>
       </c>
       <c r="B35">
-        <v>44</v>
+        <v>92</v>
       </c>
     </row>
     <row r="36">
       <c r="A36">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="B36">
-        <v>47</v>
+        <v>95</v>
       </c>
     </row>
     <row r="37">
       <c r="A37">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="B37">
-        <v>49</v>
+        <v>97</v>
       </c>
     </row>
     <row r="38">
       <c r="A38">
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="B38">
-        <v>52</v>
+        <v>100</v>
       </c>
     </row>
     <row r="39">
       <c r="A39">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="B39">
-        <v>54</v>
+        <v>102</v>
       </c>
     </row>
     <row r="40">
       <c r="A40">
-        <v>18</v>
+        <v>38</v>
       </c>
       <c r="B40">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41">
-        <v>19</v>
-      </c>
-      <c r="B41">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42">
-        <v>20</v>
-      </c>
-      <c r="B42">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43">
-        <v>21</v>
-      </c>
-      <c r="B43">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44">
-        <v>22</v>
-      </c>
-      <c r="B44">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45">
-        <v>23</v>
-      </c>
-      <c r="B45">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46">
-        <v>24</v>
-      </c>
-      <c r="B46">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47">
-        <v>25</v>
-      </c>
-      <c r="B47">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48">
-        <v>26</v>
-      </c>
-      <c r="B48">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49">
-        <v>27</v>
-      </c>
-      <c r="B49">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50">
-        <v>28</v>
-      </c>
-      <c r="B50">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51">
-        <v>29</v>
-      </c>
-      <c r="B51">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52">
-        <v>30</v>
-      </c>
-      <c r="B52">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53">
-        <v>31</v>
-      </c>
-      <c r="B53">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54">
-        <v>32</v>
-      </c>
-      <c r="B54">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55">
-        <v>33</v>
-      </c>
-      <c r="B55">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56">
-        <v>34</v>
-      </c>
-      <c r="B56">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57">
-        <v>35</v>
-      </c>
-      <c r="B57">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58">
-        <v>36</v>
-      </c>
-      <c r="B58">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59">
-        <v>37</v>
-      </c>
-      <c r="B59">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60">
-        <v>38</v>
-      </c>
-      <c r="B60">
         <v>105</v>
       </c>
     </row>

</xml_diff>